<commit_message>
Add button tambah cicilan & fix impor pembayaran
</commit_message>
<xml_diff>
--- a/public/template_pembayaran.xlsx
+++ b/public/template_pembayaran.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\web_basada\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBC560C5-D177-4FD6-B7E9-A01D6DA8BC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8388819F-4DEC-49EC-9E67-8C16FF7BA68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7C447FE9-9C64-41D9-8582-37429A9077E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{7C447FE9-9C64-41D9-8582-37429A9077E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tempalat Pembayaran" sheetId="1" r:id="rId1"/>
     <sheet name="Template Pembayaran Bulanan" sheetId="2" r:id="rId2"/>
+    <sheet name="Template Cicilan Lebih dari 1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t>nis</t>
   </si>
@@ -100,13 +101,31 @@
   </si>
   <si>
     <t>2024-12-04</t>
+  </si>
+  <si>
+    <t>nominal_cicilan_1</t>
+  </si>
+  <si>
+    <t>tanggal_bayar_1</t>
+  </si>
+  <si>
+    <t>nominal_cicilan_2</t>
+  </si>
+  <si>
+    <t>tanggal_bayar_2</t>
+  </si>
+  <si>
+    <t>2025-02-03</t>
+  </si>
+  <si>
+    <t>2024-12-09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +138,18 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,11 +172,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,13 +516,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E344C5F-F633-49EF-9BD5-D70130AB78B2}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -511,7 +545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>10522</v>
       </c>
@@ -530,7 +564,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>10522</v>
       </c>
@@ -551,7 +585,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>10522</v>
       </c>
@@ -585,12 +619,12 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>10524</v>
       </c>
@@ -637,7 +671,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>10524</v>
       </c>
@@ -659,6 +693,102 @@
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADBEB1E-DD5B-4782-A20A-76587494A990}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="5">
+        <v>10525</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5">
+        <v>10000</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="5">
+        <v>10525</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4">
+        <v>20000</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>